<commit_message>
Added an option to role for names
</commit_message>
<xml_diff>
--- a/gold.xlsx
+++ b/gold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amypo\PycharmProjects\forgagingDnDProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8627EBD2-52E4-4020-AB0D-82C1C818471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C330C95-C9A0-4FBA-A7B9-8F2F2EB1CA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6B914D8F-A235-47C2-9947-9868FBFD0AA0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
   <si>
     <t>0 GP</t>
   </si>
@@ -98,9 +98,6 @@
     <t>3 apples</t>
   </si>
   <si>
-    <t>sandels</t>
-  </si>
-  <si>
     <t>worn shirt</t>
   </si>
   <si>
@@ -279,6 +276,21 @@
   </si>
   <si>
     <t>tomato</t>
+  </si>
+  <si>
+    <t>stones</t>
+  </si>
+  <si>
+    <t>agate (blue)</t>
+  </si>
+  <si>
+    <t>quartz (clear)</t>
+  </si>
+  <si>
+    <t>sandals</t>
+  </si>
+  <si>
+    <t>rotten carrot</t>
   </si>
 </sst>
 </file>
@@ -650,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9BF776-7D9E-4FB7-A713-E1DB88F57196}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -665,7 +677,7 @@
     <col min="6" max="6" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -676,16 +688,19 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -696,16 +711,19 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -713,19 +731,22 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -733,19 +754,22 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -753,19 +777,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -773,19 +797,19 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -793,19 +817,19 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -813,19 +837,19 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -833,19 +857,19 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -853,19 +877,19 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -873,19 +897,19 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -893,19 +917,19 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -913,19 +937,19 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -933,19 +957,19 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -953,19 +977,19 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -973,16 +997,16 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -993,16 +1017,16 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1013,16 +1037,16 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1033,16 +1057,16 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1053,16 +1077,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1073,16 +1097,16 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
         <v>77</v>
-      </c>
-      <c r="F21" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>